<commit_message>
break even iemand nakijken aub
</commit_message>
<xml_diff>
--- a/Ontwikkelingstraject/Kostenberekening en monetisation.xlsx
+++ b/Ontwikkelingstraject/Kostenberekening en monetisation.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13395" windowHeight="7500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13395" windowHeight="7500" tabRatio="827" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Kostprijs werkuren" sheetId="1" r:id="rId1"/>
     <sheet name="Kostenposten" sheetId="2" r:id="rId2"/>
     <sheet name="Inkomstenmodellen" sheetId="3" r:id="rId3"/>
-    <sheet name="Break-Even" sheetId="4" r:id="rId4"/>
+    <sheet name="Break-Even schatting" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="94">
   <si>
     <t>Team</t>
   </si>
@@ -224,9 +224,6 @@
     <t>Verwarming, water, elektriciteit</t>
   </si>
   <si>
-    <t xml:space="preserve">Totaal op jaarbasis: </t>
-  </si>
-  <si>
     <t>Geschatte kostprijs project:</t>
   </si>
   <si>
@@ -282,15 +279,46 @@
   </si>
   <si>
     <t>Gratis/premium-model</t>
+  </si>
+  <si>
+    <t>Totaal jaar 1</t>
+  </si>
+  <si>
+    <t>Totaal jaar 2,3,…</t>
+  </si>
+  <si>
+    <t>Gebruikers</t>
+  </si>
+  <si>
+    <t>Vaste kosten</t>
+  </si>
+  <si>
+    <t>Omzet / gebruiker</t>
+  </si>
+  <si>
+    <t>Inkomsten</t>
+  </si>
+  <si>
+    <t>Uitgaven</t>
+  </si>
+  <si>
+    <t>Winst</t>
+  </si>
+  <si>
+    <t>Break even punt</t>
+  </si>
+  <si>
+    <t>gebruikers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="6" formatCode="&quot;€&quot;\ #,##0;[Red]&quot;€&quot;\ \-#,##0"/>
     <numFmt numFmtId="8" formatCode="&quot;€&quot;\ #,##0.00;[Red]&quot;€&quot;\ \-#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="&quot;€&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -477,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -491,28 +519,37 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="1" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -835,7 +872,7 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,13 +989,13 @@
       <c r="F10" t="s">
         <v>1</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="31">
         <v>50</v>
       </c>
       <c r="H10">
         <v>105</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="31">
         <f>G10*H10</f>
         <v>5250</v>
       </c>
@@ -973,13 +1010,13 @@
       <c r="F11" t="s">
         <v>2</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="31">
         <v>50</v>
       </c>
       <c r="H11">
         <v>105</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="31">
         <f>G11*H11</f>
         <v>5250</v>
       </c>
@@ -994,13 +1031,13 @@
       <c r="F12" t="s">
         <v>3</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="31">
         <v>80</v>
       </c>
       <c r="H12">
         <v>105</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="31">
         <f>G12*H12</f>
         <v>8400</v>
       </c>
@@ -1015,13 +1052,13 @@
       <c r="F13" t="s">
         <v>4</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="31">
         <v>80</v>
       </c>
       <c r="H13">
         <v>105</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="42">
         <f>G13*H13</f>
         <v>8400</v>
       </c>
@@ -1033,10 +1070,11 @@
       <c r="C14" s="5">
         <v>20</v>
       </c>
+      <c r="G14" s="31"/>
       <c r="H14" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="31">
         <f>SUM(I10:I13)</f>
         <v>27300</v>
       </c>
@@ -1049,11 +1087,13 @@
         <f>C10+C11+C12+C13+C14</f>
         <v>85</v>
       </c>
+      <c r="I15" s="31"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="I16" s="31"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
@@ -1062,10 +1102,10 @@
       <c r="C17">
         <v>14</v>
       </c>
-      <c r="F17" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="G17" s="20">
+      <c r="F17" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="17">
         <v>27300</v>
       </c>
     </row>
@@ -1328,10 +1368,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1343,137 +1383,211 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="18"/>
+      <c r="D1" s="38"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="31">
         <v>1500</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="31">
         <f>12*B2</f>
         <v>18000</v>
       </c>
+      <c r="D2" s="31"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="31">
         <v>100</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="31">
         <v>1200</v>
       </c>
+      <c r="D3" s="31"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="31">
         <v>1000</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="31">
         <v>12000</v>
       </c>
+      <c r="D4" s="31"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="31">
         <v>150</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="31">
         <f>12*B5</f>
         <v>1800</v>
       </c>
+      <c r="D5" s="31"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>68</v>
-      </c>
+      <c r="A6" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="32">
         <v>80</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="32">
         <v>960</v>
       </c>
+      <c r="D7" s="31"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8">
+      <c r="A8" s="31"/>
+      <c r="B8" s="31">
         <f>SUM(B2:B7)</f>
         <v>2830</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="31">
         <f>SUM(C2:C7)</f>
         <v>33960</v>
       </c>
+      <c r="D8" s="31"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="11"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="41"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="31">
         <v>300</v>
       </c>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12">
+      <c r="A12" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="31">
         <v>1000</v>
       </c>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="42">
         <v>1000</v>
       </c>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14">
+      <c r="A14" s="31"/>
+      <c r="B14" s="31">
         <f>SUM(B11:B13)</f>
         <v>2300</v>
       </c>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="31"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" s="19">
+      <c r="A16" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="43">
         <f>C8+B14</f>
         <v>36260</v>
       </c>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="31"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="43">
+        <f>C8</f>
+        <v>33960</v>
+      </c>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="31"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="31"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="31"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="31"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1485,8 +1599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1502,101 +1616,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="I1" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="J1" s="28"/>
+      <c r="A1" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="I1" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="J1" s="26"/>
       <c r="K1" s="6"/>
       <c r="L1" s="11"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="I2" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="J2" s="30">
+      <c r="I2" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" s="36">
         <f>C6</f>
-        <v>6750</v>
-      </c>
-      <c r="K2" s="24"/>
+        <v>9000</v>
+      </c>
+      <c r="K2" s="21"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3">
-        <v>35000</v>
-      </c>
-      <c r="I3" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="J3" s="32">
+        <v>50000</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" s="35">
         <f>D14</f>
         <v>21542</v>
       </c>
-      <c r="K3" s="24"/>
+      <c r="K3" s="21"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4">
         <v>10000</v>
       </c>
-      <c r="I4" s="34" t="s">
+      <c r="I4" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="33">
+      <c r="J4" s="34">
         <f>J2+J3</f>
-        <v>28292</v>
-      </c>
-      <c r="K4" s="24"/>
+        <v>30542</v>
+      </c>
+      <c r="K4" s="21"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5">
         <v>50</v>
       </c>
-      <c r="D5" s="24"/>
+      <c r="D5" s="21"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="31">
         <f>C2 *(C3+C4)*C5</f>
-        <v>6750</v>
+        <v>9000</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
+      <c r="A9" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>15</v>
@@ -1609,71 +1723,74 @@
       <c r="B11">
         <v>5000</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="20">
         <v>2.99</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="31">
         <f>B11*C11</f>
         <v>14950.000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12">
         <v>800</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="20">
         <v>1.99</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="31">
         <f>B12*C12</f>
         <v>1592</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" s="26">
+        <v>77</v>
+      </c>
+      <c r="B13" s="24">
         <v>10000000</v>
       </c>
       <c r="C13" s="5">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="32">
         <f>B13*C13</f>
         <v>5000</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D14" s="24">
+      <c r="A14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="33">
         <f>SUM(D11:D13)</f>
         <v>21542</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
-        <v>78</v>
+      <c r="A19" s="22" t="s">
+        <v>77</v>
       </c>
       <c r="B19" s="3"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B20" s="14" t="s">
+      <c r="A20" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1681,7 +1798,7 @@
       <c r="A21">
         <v>5000</v>
       </c>
-      <c r="B21" s="23">
+      <c r="B21" s="20">
         <v>4.99</v>
       </c>
     </row>
@@ -1689,7 +1806,7 @@
       <c r="A22" s="11">
         <v>10000</v>
       </c>
-      <c r="B22" s="23">
+      <c r="B22" s="20">
         <v>7.99</v>
       </c>
     </row>
@@ -1697,7 +1814,7 @@
       <c r="A23">
         <v>25000</v>
       </c>
-      <c r="B23" s="23">
+      <c r="B23" s="20">
         <v>14.99</v>
       </c>
     </row>
@@ -1705,7 +1822,7 @@
       <c r="A24">
         <v>50000</v>
       </c>
-      <c r="B24" s="23">
+      <c r="B24" s="20">
         <v>24.99</v>
       </c>
     </row>
@@ -1713,7 +1830,7 @@
       <c r="A25">
         <v>100000</v>
       </c>
-      <c r="B25" s="23">
+      <c r="B25" s="20">
         <v>34.99</v>
       </c>
     </row>
@@ -1725,12 +1842,256 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="16"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="16">
+        <f>Kostenposten!B16 + 'Kostprijs werkuren'!G17</f>
+        <v>63560</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="31">
+        <f>Inkomstenmodellen!J4/Inkomstenmodellen!C3</f>
+        <v>0.61084000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="30">
+        <f>B3/B4</f>
+        <v>104053.43461462903</v>
+      </c>
+      <c r="C5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11" s="31">
+        <v>0</v>
+      </c>
+      <c r="C11" s="16">
+        <f>B3</f>
+        <v>63560</v>
+      </c>
+      <c r="D11" s="16">
+        <f>B11-C11</f>
+        <v>-63560</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="23">
+        <v>30000</v>
+      </c>
+      <c r="B12" s="31">
+        <f>A12*B4</f>
+        <v>18325.2</v>
+      </c>
+      <c r="C12" s="16">
+        <f>B3</f>
+        <v>63560</v>
+      </c>
+      <c r="D12" s="16">
+        <f>B12-C12</f>
+        <v>-45234.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="23">
+        <v>60000</v>
+      </c>
+      <c r="B13" s="31">
+        <f>A13*B4</f>
+        <v>36650.400000000001</v>
+      </c>
+      <c r="C13" s="16">
+        <f>B3</f>
+        <v>63560</v>
+      </c>
+      <c r="D13" s="16">
+        <f>B13-C13</f>
+        <v>-26909.599999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="23">
+        <v>90000</v>
+      </c>
+      <c r="B14" s="31">
+        <f>A14*B4</f>
+        <v>54975.600000000006</v>
+      </c>
+      <c r="C14" s="16">
+        <f>B3</f>
+        <v>63560</v>
+      </c>
+      <c r="D14" s="16">
+        <f>B14-C13</f>
+        <v>-8584.3999999999942</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="23">
+        <v>120000</v>
+      </c>
+      <c r="B15" s="31">
+        <f>A15*B4</f>
+        <v>73300.800000000003</v>
+      </c>
+      <c r="C15" s="16">
+        <f>B3</f>
+        <v>63560</v>
+      </c>
+      <c r="D15" s="16">
+        <f>B15-C15</f>
+        <v>9740.8000000000029</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="23">
+        <v>150000</v>
+      </c>
+      <c r="B16" s="31">
+        <f>A16*B4</f>
+        <v>91626.000000000015</v>
+      </c>
+      <c r="C16" s="16">
+        <f>B3</f>
+        <v>63560</v>
+      </c>
+      <c r="D16" s="16">
+        <f>B16-C16</f>
+        <v>28066.000000000015</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="23">
+        <v>180000</v>
+      </c>
+      <c r="B17" s="31">
+        <f>A17*B4</f>
+        <v>109951.20000000001</v>
+      </c>
+      <c r="C17" s="16">
+        <f>B3</f>
+        <v>63560</v>
+      </c>
+      <c r="D17" s="16">
+        <f>B17-C17</f>
+        <v>46391.200000000012</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="23">
+        <v>210000</v>
+      </c>
+      <c r="B18" s="31">
+        <f>A18*B4</f>
+        <v>128276.40000000001</v>
+      </c>
+      <c r="C18" s="16">
+        <f>B3</f>
+        <v>63560</v>
+      </c>
+      <c r="D18" s="16">
+        <f>B18-C18</f>
+        <v>64716.400000000009</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="23">
+        <v>240000</v>
+      </c>
+      <c r="B19" s="31">
+        <f>A19*B4</f>
+        <v>146601.60000000001</v>
+      </c>
+      <c r="C19" s="16">
+        <f>B3</f>
+        <v>63560</v>
+      </c>
+      <c r="D19" s="16">
+        <f>B19-C19</f>
+        <v>83041.600000000006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="23">
+        <v>270000</v>
+      </c>
+      <c r="B20" s="31">
+        <f>A20*B4</f>
+        <v>164926.80000000002</v>
+      </c>
+      <c r="C20" s="16">
+        <f>B3</f>
+        <v>63560</v>
+      </c>
+      <c r="D20" s="16">
+        <f>B20-C20</f>
+        <v>101366.80000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="23">
+        <v>300000</v>
+      </c>
+      <c r="B21" s="31">
+        <f>A21*B4</f>
+        <v>183252.00000000003</v>
+      </c>
+      <c r="C21" s="16">
+        <f>B3</f>
+        <v>63560</v>
+      </c>
+      <c r="D21" s="16">
+        <f>B21-C21</f>
+        <v>119692.00000000003</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>